<commit_message>
modified:   01_Project management/0 Integration management/Bid.doc 	modified:   01_Project management/0 Integration management/Project Proposal_ V1.4.docx 	modified:   01_Project management/1 Requirement management/Requirment tracking matrix.xlsx 	deleted:    01_Project management/7 Human resource management/13.CVs -Cong.docx 	new file:   01_Project management/7 Human resource management/Cong Shang Resume V4.5.5.docx
</commit_message>
<xml_diff>
--- a/01_Project management/1 Requirement management/Requirment tracking matrix.xlsx
+++ b/01_Project management/1 Requirement management/Requirment tracking matrix.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\项目文档\01_PM\1 Requirement management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\0_Project document-20210505T043744Z-001\CharityOnlineStore\01_Project management\1 Requirement management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED78609-D8A6-4C54-8B24-D211FD73249E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5C9040-283B-46F7-87BA-3BE84F864A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-1875" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name=" Matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="requirement description" sheetId="3" r:id="rId2"/>
-    <sheet name="Index" sheetId="4" r:id="rId3"/>
+    <sheet name="Index" sheetId="4" r:id="rId1"/>
+    <sheet name=" Matrix" sheetId="1" r:id="rId2"/>
+    <sheet name="requirement description" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">' Matrix'!$E$5:$N$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">' Matrix'!$E$5:$N$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1198,11 +1198,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A60B5D-4147-4BCA-A80D-F3D3D5720950}">
+  <dimension ref="D9:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="28"/>
+    <col min="4" max="4" width="17.90625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="20.08984375" style="28" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" style="28" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D10" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D11" s="31">
+        <v>43910</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D12" s="33"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D13" s="33"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D14" s="33"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E3:N34"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K31" activeCellId="1" sqref="K30 K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1650,7 +1720,7 @@
         <v>48</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>41</v>
@@ -1678,7 +1748,7 @@
         <v>48</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>41</v>
@@ -1970,7 +2040,7 @@
         <v>47</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>41</v>
@@ -1998,7 +2068,7 @@
         <v>48</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>41</v>
@@ -2083,12 +2153,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921139E9-0F4A-4EB3-8927-BCCDC9150282}">
   <dimension ref="B3:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2527,74 +2597,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A60B5D-4147-4BCA-A80D-F3D3D5720950}">
-  <dimension ref="D9:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="3" width="8.7265625" style="28"/>
-    <col min="4" max="4" width="17.90625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" style="28" customWidth="1"/>
-    <col min="6" max="6" width="20.08984375" style="28" customWidth="1"/>
-    <col min="7" max="7" width="24.1796875" style="28" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="28"/>
-  </cols>
-  <sheetData>
-    <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D10" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D11" s="31">
-        <v>43910</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D12" s="33"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D13" s="33"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-    </row>
-    <row r="14" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D14" s="33"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>